<commit_message>
Last years (2024) ELE302 lab project.
</commit_message>
<xml_diff>
--- a/ELE302Lab/BOM_ELE302Lab.xlsx
+++ b/ELE302Lab/BOM_ELE302Lab.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dagak\GitHub\hardware\ELE302Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F54C0493-A2A6-4A78-803D-C506834DEE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788940DE-7E99-4C4B-B6A4-23F291B6B600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="735" windowWidth="33480" windowHeight="18705" xr2:uid="{64F140D1-CE97-47F7-A5E4-100946546640}"/>
+    <workbookView xWindow="57030" yWindow="1950" windowWidth="27870" windowHeight="15375" xr2:uid="{64F140D1-CE97-47F7-A5E4-100946546640}"/>
   </bookViews>
   <sheets>
     <sheet name="ELE302Lab" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1068,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E39375C-87E5-463D-AA01-77300669C3A7}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1444,12 @@
         <v>54</v>
       </c>
     </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>SUM(G9:G19)</f>
+        <v>150.19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I12" r:id="rId1" xr:uid="{AA96555D-86DC-47A3-A2F1-18E94CC6EB83}"/>

</xml_diff>